<commit_message>
added 'Deprecated' warehouse transaction type, added num_of_family_members, social_status and address for beneficiares, modified beneficiary excel example file to let social_status column be a value from a pre-defined list
</commit_message>
<xml_diff>
--- a/public/assets/templates/BeneficiariesFileTemplate.xlsx
+++ b/public/assets/templates/BeneficiariesFileTemplate.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ahmad\Humanitarian-aid-distribution-system\backend\public\assets\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Killua\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707874DF-22F3-47E0-85B7-CB6992812F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>#</t>
   </si>
@@ -66,11 +65,20 @@
   <si>
     <t>ملاحظات</t>
   </si>
+  <si>
+    <t>عدد أفراد الأسرة</t>
+  </si>
+  <si>
+    <t>الحالة الإجتماعية</t>
+  </si>
+  <si>
+    <t>عنوان السكن</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -167,7 +175,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{E7917322-F448-412C-BD9D-22940FCF1F95}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -444,11 +452,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,15 +464,18 @@
     <col min="1" max="1" width="4.21875" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
     <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" customWidth="1"/>
+    <col min="10" max="10" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,13 +498,27 @@
         <v>1</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576">
+      <formula1>"اعزب,متزوج,مطلق,ارملة"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>